<commit_message>
fixing the excel for docs
</commit_message>
<xml_diff>
--- a/doc/examples/data.xlsx
+++ b/doc/examples/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/mint/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/mint/doc/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DB604C-3C3B-B04A-92A5-199F7166C2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98314515-84D7-464D-9CEB-BDEC22A3316D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -56,12 +56,6 @@
     <t>VarA</t>
   </si>
   <si>
-    <t>Value 2</t>
-  </si>
-  <si>
-    <t>Array</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -77,33 +71,6 @@
     <t>A Variant</t>
   </si>
   <si>
-    <t>SerialNumber</t>
-  </si>
-  <si>
-    <t>FWVersionMajor</t>
-  </si>
-  <si>
-    <t>FWVersionMinor</t>
-  </si>
-  <si>
-    <t>FWVersionPatch</t>
-  </si>
-  <si>
-    <t>WiFiSSID</t>
-  </si>
-  <si>
-    <t>mynetworkname</t>
-  </si>
-  <si>
-    <t>WiFiKey</t>
-  </si>
-  <si>
-    <t>averyveryverylongstring</t>
-  </si>
-  <si>
-    <t>Coefficients1D</t>
-  </si>
-  <si>
     <t>Coefficients</t>
   </si>
   <si>
@@ -113,60 +80,15 @@
     <t>y</t>
   </si>
   <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>The rest of these will get padded out</t>
   </si>
   <si>
     <t>Keep comments at least one line away from the table</t>
   </si>
   <si>
-    <t>Block2Description</t>
-  </si>
-  <si>
-    <t>A default descripton</t>
-  </si>
-  <si>
-    <t>A debug description</t>
-  </si>
-  <si>
-    <t>BootCount</t>
-  </si>
-  <si>
-    <t>TemperatureMin</t>
-  </si>
-  <si>
-    <t>TemperatureMax</t>
-  </si>
-  <si>
-    <t>VoltageThresholds</t>
-  </si>
-  <si>
     <t>Thresholds</t>
   </si>
   <si>
-    <t>LegalNotice</t>
-  </si>
-  <si>
-    <t>Don't steal me!</t>
-  </si>
-  <si>
-    <t>CalibrationMatrix</t>
-  </si>
-  <si>
-    <t>AStructs</t>
-  </si>
-  <si>
-    <t>#Thresholds</t>
-  </si>
-  <si>
-    <t>#AnArray</t>
-  </si>
-  <si>
-    <t>#StructArray</t>
-  </si>
-  <si>
     <t>#CalibrationMatrix</t>
   </si>
   <si>
@@ -176,34 +98,19 @@
     <t>#DebugCoefficients</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>BitmapTestCount</t>
-  </si>
-  <si>
-    <t>AllowDebug</t>
-  </si>
-  <si>
-    <t>ModeSelect</t>
-  </si>
-  <si>
     <t>RegionCode</t>
   </si>
   <si>
-    <t>PowerGood</t>
-  </si>
-  <si>
-    <t>FanRunning</t>
-  </si>
-  <si>
-    <t>ErrorCode</t>
-  </si>
-  <si>
-    <t>HwRevision</t>
-  </si>
-  <si>
-    <t>BitmapCheckVal</t>
+    <t>EnableDebug</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>Version</t>
   </si>
 </sst>
 </file>
@@ -249,7 +156,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81175D9F-030E-4648-B932-899D2D945A10}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,260 +517,71 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="b">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>100600</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>12</v>
+      <c r="A6" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22">
-        <v>100</v>
-      </c>
-      <c r="D22">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23">
-        <v>-30</v>
-      </c>
-      <c r="C23">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24">
-        <v>50</v>
-      </c>
-      <c r="C24">
-        <v>60</v>
-      </c>
-      <c r="D24">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="2">
-        <v>305419896</v>
+        <v>1006</v>
       </c>
     </row>
   </sheetData>
@@ -873,17 +591,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D3322D-BF46-7347-8CBD-55E083687702}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -904,26 +622,6 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8.8000000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +641,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -973,56 +671,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308DF289-3F51-0D46-B1D3-E8F6B2D4D4A5}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1042,13 +720,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1117,7 +795,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1137,10 +815,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1240,7 +918,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixing the excel for docs (#22)
</commit_message>
<xml_diff>
--- a/doc/examples/data.xlsx
+++ b/doc/examples/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/mint/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomford/code/projects/mint/doc/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DB604C-3C3B-B04A-92A5-199F7166C2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98314515-84D7-464D-9CEB-BDEC22A3316D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" xr2:uid="{7DE5358D-EB7B-2445-85B8-580B8690A605}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -56,12 +56,6 @@
     <t>VarA</t>
   </si>
   <si>
-    <t>Value 2</t>
-  </si>
-  <si>
-    <t>Array</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -77,33 +71,6 @@
     <t>A Variant</t>
   </si>
   <si>
-    <t>SerialNumber</t>
-  </si>
-  <si>
-    <t>FWVersionMajor</t>
-  </si>
-  <si>
-    <t>FWVersionMinor</t>
-  </si>
-  <si>
-    <t>FWVersionPatch</t>
-  </si>
-  <si>
-    <t>WiFiSSID</t>
-  </si>
-  <si>
-    <t>mynetworkname</t>
-  </si>
-  <si>
-    <t>WiFiKey</t>
-  </si>
-  <si>
-    <t>averyveryverylongstring</t>
-  </si>
-  <si>
-    <t>Coefficients1D</t>
-  </si>
-  <si>
     <t>Coefficients</t>
   </si>
   <si>
@@ -113,60 +80,15 @@
     <t>y</t>
   </si>
   <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>The rest of these will get padded out</t>
   </si>
   <si>
     <t>Keep comments at least one line away from the table</t>
   </si>
   <si>
-    <t>Block2Description</t>
-  </si>
-  <si>
-    <t>A default descripton</t>
-  </si>
-  <si>
-    <t>A debug description</t>
-  </si>
-  <si>
-    <t>BootCount</t>
-  </si>
-  <si>
-    <t>TemperatureMin</t>
-  </si>
-  <si>
-    <t>TemperatureMax</t>
-  </si>
-  <si>
-    <t>VoltageThresholds</t>
-  </si>
-  <si>
     <t>Thresholds</t>
   </si>
   <si>
-    <t>LegalNotice</t>
-  </si>
-  <si>
-    <t>Don't steal me!</t>
-  </si>
-  <si>
-    <t>CalibrationMatrix</t>
-  </si>
-  <si>
-    <t>AStructs</t>
-  </si>
-  <si>
-    <t>#Thresholds</t>
-  </si>
-  <si>
-    <t>#AnArray</t>
-  </si>
-  <si>
-    <t>#StructArray</t>
-  </si>
-  <si>
     <t>#CalibrationMatrix</t>
   </si>
   <si>
@@ -176,34 +98,19 @@
     <t>#DebugCoefficients</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>BitmapTestCount</t>
-  </si>
-  <si>
-    <t>AllowDebug</t>
-  </si>
-  <si>
-    <t>ModeSelect</t>
-  </si>
-  <si>
     <t>RegionCode</t>
   </si>
   <si>
-    <t>PowerGood</t>
-  </si>
-  <si>
-    <t>FanRunning</t>
-  </si>
-  <si>
-    <t>ErrorCode</t>
-  </si>
-  <si>
-    <t>HwRevision</t>
-  </si>
-  <si>
-    <t>BitmapCheckVal</t>
+    <t>EnableDebug</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>Version</t>
   </si>
 </sst>
 </file>
@@ -249,7 +156,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81175D9F-030E-4648-B932-899D2D945A10}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,260 +517,71 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="b">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>100600</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>12</v>
+      <c r="A6" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22">
-        <v>100</v>
-      </c>
-      <c r="D22">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23">
-        <v>-30</v>
-      </c>
-      <c r="C23">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24">
-        <v>50</v>
-      </c>
-      <c r="C24">
-        <v>60</v>
-      </c>
-      <c r="D24">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34">
-        <v>-8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>50</v>
-      </c>
-      <c r="B36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="2">
-        <v>305419896</v>
+        <v>1006</v>
       </c>
     </row>
   </sheetData>
@@ -873,17 +591,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5D3322D-BF46-7347-8CBD-55E083687702}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -904,26 +622,6 @@
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8.8000000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -943,7 +641,7 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -973,56 +671,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308DF289-3F51-0D46-B1D3-E8F6B2D4D4A5}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1042,13 +720,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1117,7 +795,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1137,10 +815,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1240,7 +918,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>